<commit_message>
update database excel file
</commit_message>
<xml_diff>
--- a/data/Charcrete_database_38.xlsx
+++ b/data/Charcrete_database_38.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="87">
   <si>
     <t>cutoff</t>
   </si>
@@ -95,9 +95,6 @@
     <t>cubic meter</t>
   </si>
   <si>
-    <t>AR</t>
-  </si>
-  <si>
     <t>GLO</t>
   </si>
   <si>
@@ -236,6 +233,12 @@
     <t>market for sand</t>
   </si>
   <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
     <t>market for plasticiser, for concrete, based on sulfonated melamine formaldehyde</t>
   </si>
   <si>
@@ -255,6 +258,42 @@
   </si>
   <si>
     <t>soil::industrial</t>
+  </si>
+  <si>
+    <t>market for cement, Portland</t>
+  </si>
+  <si>
+    <t>cement, Portland</t>
+  </si>
+  <si>
+    <t>0,15739</t>
+  </si>
+  <si>
+    <t>0,047136</t>
+  </si>
+  <si>
+    <t>0,01</t>
+  </si>
+  <si>
+    <t>0,108</t>
+  </si>
+  <si>
+    <t>0,198</t>
+  </si>
+  <si>
+    <t>2,70</t>
+  </si>
+  <si>
+    <t>18,3</t>
+  </si>
+  <si>
+    <t>0,185</t>
+  </si>
+  <si>
+    <t>4,37</t>
+  </si>
+  <si>
+    <t>325,6</t>
   </si>
 </sst>
 </file>
@@ -607,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC69"/>
+  <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,25 +677,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -684,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="2">
         <v>3</v>
@@ -763,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -779,7 +818,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -828,59 +867,59 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
         <v>22</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>23</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>25</v>
       </c>
-      <c r="M11" t="s">
-        <v>26</v>
-      </c>
       <c r="P11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U11" s="4"/>
       <c r="V11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="X11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="Y11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Z11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z11" s="4" t="s">
+      <c r="AA11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA11" s="4" t="s">
+      <c r="AB11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB11" s="5" t="s">
+      <c r="AC11" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
@@ -893,16 +932,16 @@
         <v>Woodchip production</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -910,22 +949,22 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13">
-        <v>0.15739</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
@@ -969,29 +1008,29 @@
         <f>SQRT((LN(V13))^2+LN(W13)^2+LN(X13)^2+LN(Y13)^2+LN(Z13)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" t="e">
         <f>LN(D13)</f>
-        <v>-1.8490284774186274</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="D14">
-        <v>4.7135999999999997E-2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
         <v>13</v>
@@ -1002,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
@@ -1027,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
@@ -1043,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
@@ -1092,59 +1131,59 @@
         <v>11</v>
       </c>
       <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
         <v>22</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>24</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>25</v>
       </c>
-      <c r="M23" t="s">
-        <v>26</v>
-      </c>
       <c r="P23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="R23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="S23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W23" s="4" t="s">
+      <c r="X23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X23" s="4" t="s">
+      <c r="Y23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y23" s="4" t="s">
+      <c r="Z23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z23" s="4" t="s">
+      <c r="AA23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA23" s="4" t="s">
+      <c r="AB23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB23" s="5" t="s">
+      <c r="AC23" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC23" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
@@ -1157,16 +1196,16 @@
         <v>Woodchip transport</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
@@ -1174,22 +1213,22 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>200</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
         <v>13</v>
@@ -1246,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
@@ -1271,7 +1310,7 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
@@ -1287,7 +1326,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
@@ -1336,59 +1375,59 @@
         <v>11</v>
       </c>
       <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
         <v>22</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>23</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>24</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>25</v>
       </c>
-      <c r="M34" t="s">
-        <v>26</v>
-      </c>
       <c r="P34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q34" s="4" t="s">
+      <c r="R34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="S34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W34" s="4" t="s">
+      <c r="X34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X34" s="4" t="s">
+      <c r="Y34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y34" s="4" t="s">
+      <c r="Z34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z34" s="4" t="s">
+      <c r="AA34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA34" s="4" t="s">
+      <c r="AB34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB34" s="5" t="s">
+      <c r="AC34" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC34" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
@@ -1401,16 +1440,16 @@
         <v>Pyrolysis</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1424,16 +1463,16 @@
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36">
-        <v>0.01</v>
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
       </c>
       <c r="E36" t="s">
         <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G36" t="s">
         <v>13</v>
@@ -1477,29 +1516,29 @@
         <f>SQRT((LN(V36))^2+LN(W36)^2+LN(X36)^2+LN(Y36)^2+LN(Z36)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB36">
+      <c r="AB36" t="e">
         <f>LN(D36)</f>
-        <v>-4.6051701859880909</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37">
-        <v>0.108</v>
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37" t="s">
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P37">
         <v>4</v>
@@ -1540,29 +1579,29 @@
         <f>SQRT((LN(V37))^2+LN(W37)^2+LN(X37)^2+LN(Y37)^2+LN(Z37)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB37">
+      <c r="AB37" t="e">
         <f>LN(D37)</f>
-        <v>-2.2256240518579173</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38">
-        <v>0.19800000000000001</v>
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>81</v>
       </c>
       <c r="E38" t="s">
         <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G38" t="s">
         <v>18</v>
       </c>
       <c r="H38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P38">
         <v>4</v>
@@ -1603,9 +1642,9 @@
         <f>SQRT((LN(V38))^2+LN(W38)^2+LN(X38)^2+LN(Y38)^2+LN(Z38)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB38">
+      <c r="AB38" t="e">
         <f>LN(D38)</f>
-        <v>-1.6194882482876019</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
@@ -1613,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
@@ -1638,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
@@ -1654,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
@@ -1703,59 +1742,59 @@
         <v>11</v>
       </c>
       <c r="I47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" t="s">
         <v>22</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>23</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>24</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>25</v>
       </c>
-      <c r="M47" t="s">
-        <v>26</v>
-      </c>
       <c r="P47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q47" s="4" t="s">
+      <c r="R47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R47" s="4" t="s">
+      <c r="S47" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S47" s="4" t="s">
+      <c r="T47" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T47" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U47" s="4"/>
       <c r="V47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W47" s="4" t="s">
+      <c r="X47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X47" s="4" t="s">
+      <c r="Y47" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y47" s="4" t="s">
+      <c r="Z47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z47" s="4" t="s">
+      <c r="AA47" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA47" s="4" t="s">
+      <c r="AB47" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB47" s="5" t="s">
+      <c r="AC47" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC47" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.3">
@@ -1768,7 +1807,7 @@
         <v>Biochar production</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1777,7 +1816,7 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G48" t="s">
         <v>12</v>
@@ -1785,23 +1824,22 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
         <v>38</v>
       </c>
-      <c r="B49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
         <v>39</v>
       </c>
-      <c r="D49">
-        <f>1/0.37</f>
-        <v>2.7027027027027026</v>
-      </c>
-      <c r="E49" t="s">
-        <v>40</v>
-      </c>
       <c r="F49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
@@ -1845,30 +1883,29 @@
         <f>SQRT((LN(V49))^2+LN(W49)^2+LN(X49)^2+LN(Y49)^2+LN(Z49)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB49">
+      <c r="AB49" t="e">
         <f>LN(D49)</f>
-        <v>0.9942522733438669</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" t="s">
         <v>39</v>
       </c>
-      <c r="D50">
-        <f t="shared" ref="D50:D51" si="9">1/0.37</f>
-        <v>2.7027027027027026</v>
-      </c>
-      <c r="E50" t="s">
-        <v>40</v>
-      </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
@@ -1912,30 +1949,29 @@
         <f>SQRT((LN(V50))^2+LN(W50)^2+LN(X50)^2+LN(Y50)^2+LN(Z50)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB50">
+      <c r="AB50" t="e">
         <f>LN(D50)</f>
-        <v>0.9942522733438669</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" t="s">
         <v>39</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="9"/>
-        <v>2.7027027027027026</v>
-      </c>
-      <c r="E51" t="s">
-        <v>40</v>
-      </c>
       <c r="F51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
@@ -1946,7 +1982,7 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.3">
@@ -1971,7 +2007,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.3">
@@ -2036,59 +2072,59 @@
         <v>11</v>
       </c>
       <c r="I60" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" t="s">
         <v>22</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
         <v>23</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>24</v>
       </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>25</v>
       </c>
-      <c r="M60" t="s">
-        <v>26</v>
-      </c>
       <c r="P60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q60" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q60" s="4" t="s">
+      <c r="R60" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R60" s="4" t="s">
+      <c r="S60" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S60" s="4" t="s">
+      <c r="T60" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T60" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U60" s="4"/>
       <c r="V60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W60" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W60" s="4" t="s">
+      <c r="X60" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X60" s="4" t="s">
+      <c r="Y60" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Y60" s="4" t="s">
+      <c r="Z60" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Z60" s="4" t="s">
+      <c r="AA60" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA60" s="4" t="s">
+      <c r="AB60" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AB60" s="5" t="s">
+      <c r="AC60" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC60" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
@@ -2101,7 +2137,7 @@
         <v>Charcrete production</v>
       </c>
       <c r="C61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2110,7 +2146,7 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G61" t="s">
         <v>12</v>
@@ -2118,23 +2154,22 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
-      </c>
-      <c r="D62">
-        <f>111/1000</f>
-        <v>0.111</v>
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>83</v>
       </c>
       <c r="E62" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G62" t="s">
         <v>13</v>
@@ -2155,43 +2190,43 @@
         <v>3</v>
       </c>
       <c r="V62">
-        <f t="shared" ref="V62" si="10">+VLOOKUP(P62, $P$2:$U$6, 2+W$10,0)</f>
+        <f t="shared" ref="V62" si="9">+VLOOKUP(P62, $P$2:$U$6, 2+W$10,0)</f>
         <v>1.2</v>
       </c>
       <c r="W62">
-        <f t="shared" ref="W62" si="11">+VLOOKUP(Q62, $P$2:$U$6, 2+X$10,0)</f>
+        <f t="shared" ref="W62" si="10">+VLOOKUP(Q62, $P$2:$U$6, 2+X$10,0)</f>
         <v>1.2</v>
       </c>
       <c r="X62">
-        <f t="shared" ref="X62" si="12">+VLOOKUP(R62, $P$2:$U$6, 2+Y$10,0)</f>
+        <f t="shared" ref="X62" si="11">+VLOOKUP(R62, $P$2:$U$6, 2+Y$10,0)</f>
         <v>1.5</v>
       </c>
       <c r="Y62">
-        <f t="shared" ref="Y62" si="13">+VLOOKUP(S62, $P$2:$U$6, 2+Z$10,0)</f>
+        <f t="shared" ref="Y62" si="12">+VLOOKUP(S62, $P$2:$U$6, 2+Z$10,0)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="Z62">
-        <f t="shared" ref="Z62" si="14">+VLOOKUP(T62, $P$2:$U$6, 2+AA$10,0)</f>
+        <f t="shared" ref="Z62" si="13">+VLOOKUP(T62, $P$2:$U$6, 2+AA$10,0)</f>
         <v>1.2</v>
       </c>
       <c r="AA62">
         <f>SQRT((LN(V62))^2+LN(W62)^2+LN(X62)^2+LN(Y62)^2+LN(Z62)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB62">
+      <c r="AB62" t="e">
         <f>LN(D62)</f>
-        <v>-2.1982250776698029</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" t="s">
         <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>57</v>
-      </c>
-      <c r="C63" t="s">
-        <v>63</v>
       </c>
       <c r="D63">
         <v>857</v>
@@ -2200,7 +2235,7 @@
         <v>16</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G63" t="s">
         <v>13</v>
@@ -2208,22 +2243,22 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" t="s">
         <v>58</v>
       </c>
-      <c r="B64" t="s">
-        <v>59</v>
-      </c>
       <c r="C64" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64">
-        <v>5.4</v>
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>66</v>
       </c>
       <c r="E64" t="s">
         <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G64" t="s">
         <v>13</v>
@@ -2231,23 +2266,22 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65">
-        <f>185/1000</f>
-        <v>0.185</v>
+      <c r="D65" t="s">
+        <v>84</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G65" t="s">
         <v>13</v>
@@ -2255,13 +2289,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D66">
         <v>857</v>
@@ -2270,7 +2304,7 @@
         <v>16</v>
       </c>
       <c r="F66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G66" t="s">
         <v>13</v>
@@ -2278,22 +2312,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67">
-        <v>4.37</v>
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>85</v>
       </c>
       <c r="E67" t="s">
         <v>16</v>
       </c>
       <c r="F67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G67" t="s">
         <v>13</v>
@@ -2301,22 +2335,22 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68">
-        <v>0.2</v>
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G68" t="s">
         <v>13</v>
@@ -2324,22 +2358,45 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="B69" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
       </c>
       <c r="D69">
-        <v>325.60000000000002</v>
+        <v>347</v>
       </c>
       <c r="E69" t="s">
         <v>16</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" t="s">
         <v>18</v>
       </c>
-      <c r="H69" t="s">
-        <v>73</v>
+      <c r="H70" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update database excel file dot style
</commit_message>
<xml_diff>
--- a/data/Charcrete_database_38.xlsx
+++ b/data/Charcrete_database_38.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="75">
   <si>
     <t>cutoff</t>
   </si>
@@ -233,12 +233,6 @@
     <t>market for sand</t>
   </si>
   <si>
-    <t>5,4</t>
-  </si>
-  <si>
-    <t>0,2</t>
-  </si>
-  <si>
     <t>market for plasticiser, for concrete, based on sulfonated melamine formaldehyde</t>
   </si>
   <si>
@@ -264,36 +258,6 @@
   </si>
   <si>
     <t>cement, Portland</t>
-  </si>
-  <si>
-    <t>0,15739</t>
-  </si>
-  <si>
-    <t>0,047136</t>
-  </si>
-  <si>
-    <t>0,01</t>
-  </si>
-  <si>
-    <t>0,108</t>
-  </si>
-  <si>
-    <t>0,198</t>
-  </si>
-  <si>
-    <t>2,70</t>
-  </si>
-  <si>
-    <t>18,3</t>
-  </si>
-  <si>
-    <t>0,185</t>
-  </si>
-  <si>
-    <t>4,37</t>
-  </si>
-  <si>
-    <t>325,6</t>
   </si>
 </sst>
 </file>
@@ -648,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -957,8 +921,8 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
-        <v>77</v>
+      <c r="D13">
+        <v>0.15739</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
@@ -1008,9 +972,9 @@
         <f>SQRT((LN(V13))^2+LN(W13)^2+LN(X13)^2+LN(Y13)^2+LN(Z13)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB13" t="e">
+      <c r="AB13">
         <f>LN(D13)</f>
-        <v>#VALUE!</v>
+        <v>-1.8490284774186274</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
@@ -1023,8 +987,8 @@
       <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="D14" t="s">
-        <v>78</v>
+      <c r="D14">
+        <v>4.7135999999999997E-2</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
@@ -1465,8 +1429,8 @@
       <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="D36" t="s">
-        <v>79</v>
+      <c r="D36">
+        <v>0.01</v>
       </c>
       <c r="E36" t="s">
         <v>17</v>
@@ -1516,17 +1480,17 @@
         <f>SQRT((LN(V36))^2+LN(W36)^2+LN(X36)^2+LN(Y36)^2+LN(Z36)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB36" t="e">
+      <c r="AB36">
         <f>LN(D36)</f>
-        <v>#VALUE!</v>
+        <v>-4.6051701859880909</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="D37" t="s">
-        <v>80</v>
+      <c r="D37">
+        <v>0.108</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
@@ -1579,17 +1543,17 @@
         <f>SQRT((LN(V37))^2+LN(W37)^2+LN(X37)^2+LN(Y37)^2+LN(Z37)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB37" t="e">
+      <c r="AB37">
         <f>LN(D37)</f>
-        <v>#VALUE!</v>
+        <v>-2.2256240518579173</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
-      <c r="D38" t="s">
-        <v>81</v>
+      <c r="D38">
+        <v>0.19800000000000001</v>
       </c>
       <c r="E38" t="s">
         <v>16</v>
@@ -1642,9 +1606,9 @@
         <f>SQRT((LN(V38))^2+LN(W38)^2+LN(X38)^2+LN(Y38)^2+LN(Z38)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB38" t="e">
+      <c r="AB38">
         <f>LN(D38)</f>
-        <v>#VALUE!</v>
+        <v>-1.6194882482876019</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
@@ -1832,8 +1796,8 @@
       <c r="C49" t="s">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
-        <v>82</v>
+      <c r="D49">
+        <v>2.7</v>
       </c>
       <c r="E49" t="s">
         <v>39</v>
@@ -1883,9 +1847,9 @@
         <f>SQRT((LN(V49))^2+LN(W49)^2+LN(X49)^2+LN(Y49)^2+LN(Z49)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB49" t="e">
+      <c r="AB49">
         <f>LN(D49)</f>
-        <v>#VALUE!</v>
+        <v>0.99325177301028345</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
@@ -1898,8 +1862,8 @@
       <c r="C50" t="s">
         <v>38</v>
       </c>
-      <c r="D50" t="s">
-        <v>82</v>
+      <c r="D50">
+        <v>2.7</v>
       </c>
       <c r="E50" t="s">
         <v>39</v>
@@ -1949,9 +1913,9 @@
         <f>SQRT((LN(V50))^2+LN(W50)^2+LN(X50)^2+LN(Y50)^2+LN(Z50)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB50" t="e">
+      <c r="AB50">
         <f>LN(D50)</f>
-        <v>#VALUE!</v>
+        <v>0.99325177301028345</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
@@ -1964,8 +1928,8 @@
       <c r="C51" t="s">
         <v>38</v>
       </c>
-      <c r="D51" t="s">
-        <v>82</v>
+      <c r="D51">
+        <v>2.7</v>
       </c>
       <c r="E51" t="s">
         <v>39</v>
@@ -2162,8 +2126,8 @@
       <c r="C62" t="s">
         <v>38</v>
       </c>
-      <c r="D62" t="s">
-        <v>83</v>
+      <c r="D62">
+        <v>18.3</v>
       </c>
       <c r="E62" t="s">
         <v>16</v>
@@ -2213,9 +2177,9 @@
         <f>SQRT((LN(V62))^2+LN(W62)^2+LN(X62)^2+LN(Y62)^2+LN(Z62)^2)</f>
         <v>0.52269439874826651</v>
       </c>
-      <c r="AB62" t="e">
+      <c r="AB62">
         <f>LN(D62)</f>
-        <v>#VALUE!</v>
+        <v>2.9069010598473755</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
@@ -2251,8 +2215,8 @@
       <c r="C64" t="s">
         <v>38</v>
       </c>
-      <c r="D64" t="s">
-        <v>66</v>
+      <c r="D64">
+        <v>5.4</v>
       </c>
       <c r="E64" t="s">
         <v>17</v>
@@ -2274,8 +2238,8 @@
       <c r="C65" t="s">
         <v>64</v>
       </c>
-      <c r="D65" t="s">
-        <v>84</v>
+      <c r="D65">
+        <v>0.185</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
@@ -2312,16 +2276,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" t="s">
         <v>20</v>
       </c>
-      <c r="D67" t="s">
-        <v>85</v>
+      <c r="D67">
+        <v>4.37</v>
       </c>
       <c r="E67" t="s">
         <v>16</v>
@@ -2335,19 +2299,19 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
         <v>20</v>
       </c>
-      <c r="D68" t="s">
-        <v>67</v>
+      <c r="D68">
+        <v>0.2</v>
       </c>
       <c r="E68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F68" t="s">
         <v>41</v>
@@ -2358,10 +2322,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
         <v>64</v>
@@ -2381,10 +2345,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>73</v>
-      </c>
-      <c r="D70" t="s">
-        <v>86</v>
+        <v>71</v>
+      </c>
+      <c r="D70">
+        <v>325.60000000000002</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>
@@ -2396,7 +2360,7 @@
         <v>18</v>
       </c>
       <c r="H70" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
charcrete 14 update biogenic
</commit_message>
<xml_diff>
--- a/data/Charcrete_database_38.xlsx
+++ b/data/Charcrete_database_38.xlsx
@@ -266,9 +266,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,8 +1625,9 @@
       <c r="A70" t="s">
         <v>60</v>
       </c>
-      <c r="D70">
-        <v>325.60000000000002</v>
+      <c r="D70" s="2">
+        <f>325.6*0.0183</f>
+        <v>5.9584800000000007</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>

</xml_diff>